<commit_message>
checkpoint for using onemaps api. switching to gmaps
</commit_message>
<xml_diff>
--- a/processed data/PPHS Summary (August 2024).xlsx
+++ b/processed data/PPHS Summary (August 2024).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yeelongsiah/Desktop/Personal/PythonLearning/PPHS/processed data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5CFBD4D-E57D-EB49-88C0-5D60EA53101F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479170C9-B04A-7648-A737-B0F373D4A106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,27 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$43</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="83">
   <si>
     <t>town</t>
   </si>
@@ -266,6 +279,12 @@
   </si>
   <si>
     <t>4Q 2026</t>
+  </si>
+  <si>
+    <t>nearest MRT score</t>
+  </si>
+  <si>
+    <t>most central score</t>
   </si>
 </sst>
 </file>
@@ -297,7 +316,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -320,13 +339,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -633,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -653,7 +686,7 @@
     <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -684,72 +717,94 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2">
+        <v>7</v>
+      </c>
+      <c r="F2">
         <v>16</v>
       </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-      <c r="F2">
-        <v>21</v>
-      </c>
       <c r="G2">
-        <v>800</v>
+        <v>550</v>
       </c>
       <c r="H2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2">
+        <v>37</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <f>IF(E2&lt;10, 1, IF(E2&lt;15,2,IF(E2&lt;20,3,4)))</f>
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <f>IF(F2&lt;20, 1, IF(F2&lt;30,2,IF(F2&lt;45,3,4)))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <v>700</v>
+      </c>
+      <c r="H3" t="s">
         <v>78</v>
       </c>
-      <c r="I2">
-        <v>64</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E3">
+      <c r="I3">
+        <v>64</v>
+      </c>
+      <c r="J3">
         <v>5</v>
       </c>
-      <c r="F3">
-        <v>20</v>
-      </c>
-      <c r="G3">
-        <v>550</v>
-      </c>
-      <c r="H3" t="s">
-        <v>79</v>
-      </c>
-      <c r="I3">
-        <v>37</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3">
+        <f>IF(E3&lt;10, 1, IF(E3&lt;15,2,IF(E3&lt;20,3,4)))</f>
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <f>IF(F3&lt;20, 1, IF(F3&lt;30,2,IF(F3&lt;45,3,4)))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -757,16 +812,16 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
         <v>64</v>
       </c>
       <c r="E4">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4">
         <v>700</v>
@@ -778,30 +833,38 @@
         <v>37</v>
       </c>
       <c r="J4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <f>IF(E4&lt;10, 1, IF(E4&lt;15,2,IF(E4&lt;20,3,4)))</f>
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <f>IF(F4&lt;20, 1, IF(F4&lt;30,2,IF(F4&lt;45,3,4)))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G5">
-        <v>550</v>
+        <v>700</v>
       </c>
       <c r="H5" t="s">
         <v>79</v>
@@ -810,62 +873,78 @@
         <v>37</v>
       </c>
       <c r="J5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <f>IF(E5&lt;10, 1, IF(E5&lt;15,2,IF(E5&lt;20,3,4)))</f>
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <f>IF(F5&lt;20, 1, IF(F5&lt;30,2,IF(F5&lt;45,3,4)))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="E6">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F6">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="G6">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="H6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I6">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="J6">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <f>IF(E6&lt;10, 1, IF(E6&lt;15,2,IF(E6&lt;20,3,4)))</f>
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <f>IF(F6&lt;20, 1, IF(F6&lt;30,2,IF(F6&lt;45,3,4)))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
         <v>64</v>
       </c>
       <c r="E7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F7">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7">
-        <v>700</v>
+        <v>1500</v>
       </c>
       <c r="H7" t="s">
         <v>79</v>
@@ -874,10 +953,18 @@
         <v>37</v>
       </c>
       <c r="J7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <f>IF(E7&lt;10, 1, IF(E7&lt;15,2,IF(E7&lt;20,3,4)))</f>
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <f>IF(F7&lt;20, 1, IF(F7&lt;30,2,IF(F7&lt;45,3,4)))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -908,57 +995,73 @@
       <c r="J8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8">
+        <f>IF(E8&lt;10, 1, IF(E8&lt;15,2,IF(E8&lt;20,3,4)))</f>
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <f>IF(F8&lt;20, 1, IF(F8&lt;30,2,IF(F8&lt;45,3,4)))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="E9">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F9">
+        <v>20</v>
+      </c>
+      <c r="G9">
+        <v>550</v>
+      </c>
+      <c r="H9" t="s">
+        <v>79</v>
+      </c>
+      <c r="I9">
+        <v>37</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <f>IF(E9&lt;10, 1, IF(E9&lt;15,2,IF(E9&lt;20,3,4)))</f>
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <f>IF(F9&lt;20, 1, IF(F9&lt;30,2,IF(F9&lt;45,3,4)))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="G9">
-        <v>700</v>
-      </c>
-      <c r="H9" t="s">
-        <v>78</v>
-      </c>
-      <c r="I9">
-        <v>64</v>
-      </c>
-      <c r="J9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
       <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10">
         <v>4</v>
       </c>
-      <c r="C10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" t="s">
-        <v>76</v>
-      </c>
-      <c r="E10">
-        <v>8</v>
-      </c>
       <c r="F10">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="G10">
         <v>800</v>
@@ -970,91 +1073,115 @@
         <v>64</v>
       </c>
       <c r="J10">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <f>IF(E10&lt;10, 1, IF(E10&lt;15,2,IF(E10&lt;20,3,4)))</f>
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <f>IF(F10&lt;20, 1, IF(F10&lt;30,2,IF(F10&lt;45,3,4)))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B11">
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="E11">
         <v>9</v>
       </c>
       <c r="F11">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="G11">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="H11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I11">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="J11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <f>IF(E11&lt;10, 1, IF(E11&lt;15,2,IF(E11&lt;20,3,4)))</f>
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <f>IF(F11&lt;20, 1, IF(F11&lt;30,2,IF(F11&lt;45,3,4)))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B12">
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="E12">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F12">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="G12">
-        <v>1500</v>
+        <v>800</v>
       </c>
       <c r="H12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I12">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="J12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="K12">
+        <f>IF(E12&lt;10, 1, IF(E12&lt;15,2,IF(E12&lt;20,3,4)))</f>
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <f>IF(F12&lt;20, 1, IF(F12&lt;30,2,IF(F12&lt;45,3,4)))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D13" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E13">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="G13">
         <v>800</v>
@@ -1066,50 +1193,66 @@
         <v>64</v>
       </c>
       <c r="J13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="K13">
+        <f>IF(E13&lt;10, 1, IF(E13&lt;15,2,IF(E13&lt;20,3,4)))</f>
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <f>IF(F13&lt;20, 1, IF(F13&lt;30,2,IF(F13&lt;45,3,4)))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="E14">
         <v>10</v>
       </c>
       <c r="F14">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G14">
-        <v>700</v>
+        <v>550</v>
       </c>
       <c r="H14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I14">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="J14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="K14">
+        <f>IF(E14&lt;10, 1, IF(E14&lt;15,2,IF(E14&lt;20,3,4)))</f>
+        <v>2</v>
+      </c>
+      <c r="L14">
+        <f>IF(F14&lt;20, 1, IF(F14&lt;30,2,IF(F14&lt;45,3,4)))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
         <v>64</v>
@@ -1118,22 +1261,30 @@
         <v>10</v>
       </c>
       <c r="F15">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G15">
-        <v>1500</v>
+        <v>700</v>
       </c>
       <c r="H15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I15">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="J15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K15">
+        <f>IF(E15&lt;10, 1, IF(E15&lt;15,2,IF(E15&lt;20,3,4)))</f>
+        <v>2</v>
+      </c>
+      <c r="L15">
+        <f>IF(F15&lt;20, 1, IF(F15&lt;30,2,IF(F15&lt;45,3,4)))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1141,16 +1292,16 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
         <v>64</v>
       </c>
       <c r="E16">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F16">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G16">
         <v>700</v>
@@ -1164,153 +1315,193 @@
       <c r="J16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16">
+        <f>IF(E16&lt;10, 1, IF(E16&lt;15,2,IF(E16&lt;20,3,4)))</f>
+        <v>2</v>
+      </c>
+      <c r="L16">
+        <f>IF(F16&lt;20, 1, IF(F16&lt;30,2,IF(F16&lt;45,3,4)))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="E17">
         <v>10</v>
       </c>
       <c r="F17">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G17">
-        <v>550</v>
+        <v>700</v>
       </c>
       <c r="H17" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I17">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="J17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="K17">
+        <f>IF(E17&lt;10, 1, IF(E17&lt;15,2,IF(E17&lt;20,3,4)))</f>
+        <v>2</v>
+      </c>
+      <c r="L17">
+        <f>IF(F17&lt;20, 1, IF(F17&lt;30,2,IF(F17&lt;45,3,4)))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E18">
         <v>10</v>
       </c>
       <c r="F18">
+        <v>11</v>
+      </c>
+      <c r="G18">
+        <v>1500</v>
+      </c>
+      <c r="H18" t="s">
+        <v>80</v>
+      </c>
+      <c r="I18">
+        <v>25</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <f>IF(E18&lt;10, 1, IF(E18&lt;15,2,IF(E18&lt;20,3,4)))</f>
+        <v>2</v>
+      </c>
+      <c r="L18">
+        <f>IF(F18&lt;20, 1, IF(F18&lt;30,2,IF(F18&lt;45,3,4)))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>23</v>
       </c>
-      <c r="G18">
-        <v>800</v>
-      </c>
-      <c r="H18" t="s">
-        <v>78</v>
-      </c>
-      <c r="I18">
-        <v>64</v>
-      </c>
-      <c r="J18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19">
         <v>13</v>
       </c>
-      <c r="B19">
-        <v>3</v>
-      </c>
-      <c r="C19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19">
-        <v>11</v>
-      </c>
       <c r="F19">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G19">
-        <v>700</v>
+        <v>550</v>
       </c>
       <c r="H19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I19">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="J19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K19">
+        <f>IF(E19&lt;10, 1, IF(E19&lt;15,2,IF(E19&lt;20,3,4)))</f>
+        <v>2</v>
+      </c>
+      <c r="L19">
+        <f>IF(F19&lt;20, 1, IF(F19&lt;30,2,IF(F19&lt;45,3,4)))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20">
+        <v>12</v>
+      </c>
+      <c r="F20">
+        <v>25</v>
+      </c>
+      <c r="G20">
+        <v>550</v>
+      </c>
+      <c r="H20" t="s">
+        <v>79</v>
+      </c>
+      <c r="I20">
+        <v>37</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <f>IF(E20&lt;10, 1, IF(E20&lt;15,2,IF(E20&lt;20,3,4)))</f>
+        <v>2</v>
+      </c>
+      <c r="L20">
+        <f>IF(F20&lt;20, 1, IF(F20&lt;30,2,IF(F20&lt;45,3,4)))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>16</v>
       </c>
-      <c r="B20">
-        <v>3</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
         <v>39</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>69</v>
-      </c>
-      <c r="E20">
-        <v>11</v>
-      </c>
-      <c r="F20">
-        <v>20</v>
-      </c>
-      <c r="G20">
-        <v>800</v>
-      </c>
-      <c r="H20" t="s">
-        <v>78</v>
-      </c>
-      <c r="I20">
-        <v>64</v>
-      </c>
-      <c r="J20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>3</v>
-      </c>
-      <c r="C21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" t="s">
-        <v>74</v>
       </c>
       <c r="E21">
         <v>11</v>
       </c>
       <c r="F21">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G21">
         <v>800</v>
@@ -1322,10 +1513,18 @@
         <v>64</v>
       </c>
       <c r="J21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="K21">
+        <f>IF(E21&lt;10, 1, IF(E21&lt;15,2,IF(E21&lt;20,3,4)))</f>
+        <v>2</v>
+      </c>
+      <c r="L21">
+        <f>IF(F21&lt;20, 1, IF(F21&lt;30,2,IF(F21&lt;45,3,4)))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1333,16 +1532,16 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D22" t="s">
         <v>74</v>
       </c>
       <c r="E22">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F22">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G22">
         <v>800</v>
@@ -1356,25 +1555,33 @@
       <c r="J22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K22">
+        <f>IF(E22&lt;10, 1, IF(E22&lt;15,2,IF(E22&lt;20,3,4)))</f>
+        <v>2</v>
+      </c>
+      <c r="L22">
+        <f>IF(F22&lt;20, 1, IF(F22&lt;30,2,IF(F22&lt;45,3,4)))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B23">
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D23" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="E23">
         <v>11</v>
       </c>
       <c r="F23">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G23">
         <v>800</v>
@@ -1386,170 +1593,218 @@
         <v>64</v>
       </c>
       <c r="J23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <f>IF(E23&lt;10, 1, IF(E23&lt;15,2,IF(E23&lt;20,3,4)))</f>
+        <v>2</v>
+      </c>
+      <c r="L23">
+        <f>IF(F23&lt;20, 1, IF(F23&lt;30,2,IF(F23&lt;45,3,4)))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24">
+        <v>11</v>
+      </c>
+      <c r="F24">
+        <v>24</v>
+      </c>
+      <c r="G24">
+        <v>800</v>
+      </c>
+      <c r="H24" t="s">
+        <v>78</v>
+      </c>
+      <c r="I24">
+        <v>64</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <f>IF(E24&lt;10, 1, IF(E24&lt;15,2,IF(E24&lt;20,3,4)))</f>
+        <v>2</v>
+      </c>
+      <c r="L24">
+        <f>IF(F24&lt;20, 1, IF(F24&lt;30,2,IF(F24&lt;45,3,4)))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B24">
-        <v>2</v>
-      </c>
-      <c r="C24" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" t="s">
         <v>23</v>
       </c>
-      <c r="E24">
+      <c r="E25">
+        <v>11</v>
+      </c>
+      <c r="F25">
+        <v>24</v>
+      </c>
+      <c r="G25">
+        <v>800</v>
+      </c>
+      <c r="H25" t="s">
+        <v>78</v>
+      </c>
+      <c r="I25">
+        <v>64</v>
+      </c>
+      <c r="J25">
+        <v>2</v>
+      </c>
+      <c r="K25">
+        <f>IF(E25&lt;10, 1, IF(E25&lt;15,2,IF(E25&lt;20,3,4)))</f>
+        <v>2</v>
+      </c>
+      <c r="L25">
+        <f>IF(F25&lt;20, 1, IF(F25&lt;30,2,IF(F25&lt;45,3,4)))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>12</v>
       </c>
-      <c r="F24">
-        <v>25</v>
-      </c>
-      <c r="G24">
-        <v>550</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26">
+        <v>14</v>
+      </c>
+      <c r="F26">
+        <v>43</v>
+      </c>
+      <c r="G26">
+        <v>700</v>
+      </c>
+      <c r="H26" t="s">
+        <v>78</v>
+      </c>
+      <c r="I26">
+        <v>64</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <f>IF(E26&lt;10, 1, IF(E26&lt;15,2,IF(E26&lt;20,3,4)))</f>
+        <v>2</v>
+      </c>
+      <c r="L26">
+        <f>IF(F26&lt;20, 1, IF(F26&lt;30,2,IF(F26&lt;45,3,4)))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" t="s">
+        <v>73</v>
+      </c>
+      <c r="E27">
+        <v>12</v>
+      </c>
+      <c r="F27">
+        <v>45</v>
+      </c>
+      <c r="G27">
+        <v>500</v>
+      </c>
+      <c r="H27" t="s">
         <v>79</v>
       </c>
-      <c r="I24">
+      <c r="I27">
         <v>37</v>
       </c>
-      <c r="J24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="J27">
+        <v>2</v>
+      </c>
+      <c r="K27">
+        <f>IF(E27&lt;10, 1, IF(E27&lt;15,2,IF(E27&lt;20,3,4)))</f>
+        <v>2</v>
+      </c>
+      <c r="L27">
+        <f>IF(F27&lt;20, 1, IF(F27&lt;30,2,IF(F27&lt;45,3,4)))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28">
         <v>18</v>
       </c>
-      <c r="B25">
-        <v>2</v>
-      </c>
-      <c r="C25" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" t="s">
-        <v>73</v>
-      </c>
-      <c r="E25">
-        <v>12</v>
-      </c>
-      <c r="F25">
-        <v>45</v>
-      </c>
-      <c r="G25">
-        <v>500</v>
-      </c>
-      <c r="H25" t="s">
-        <v>79</v>
-      </c>
-      <c r="I25">
-        <v>37</v>
-      </c>
-      <c r="J25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26">
-        <v>2</v>
-      </c>
-      <c r="C26" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" t="s">
-        <v>75</v>
-      </c>
-      <c r="E26">
-        <v>13</v>
-      </c>
-      <c r="F26">
-        <v>24</v>
-      </c>
-      <c r="G26">
-        <v>550</v>
-      </c>
-      <c r="H26" t="s">
-        <v>79</v>
-      </c>
-      <c r="I26">
-        <v>37</v>
-      </c>
-      <c r="J26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27">
-        <v>3</v>
-      </c>
-      <c r="C27" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27">
-        <v>14</v>
-      </c>
-      <c r="F27">
-        <v>43</v>
-      </c>
-      <c r="G27">
-        <v>700</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="F28">
+        <v>27</v>
+      </c>
+      <c r="G28">
+        <v>800</v>
+      </c>
+      <c r="H28" t="s">
         <v>78</v>
       </c>
-      <c r="I27">
-        <v>64</v>
-      </c>
-      <c r="J27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28">
-        <v>2</v>
-      </c>
-      <c r="C28" t="s">
-        <v>37</v>
-      </c>
-      <c r="D28" t="s">
-        <v>67</v>
-      </c>
-      <c r="E28">
-        <v>15</v>
-      </c>
-      <c r="F28">
-        <v>50</v>
-      </c>
-      <c r="G28">
-        <v>400</v>
-      </c>
-      <c r="H28" t="s">
-        <v>79</v>
-      </c>
       <c r="I28">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="J28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <f>IF(E28&lt;10, 1, IF(E28&lt;15,2,IF(E28&lt;20,3,4)))</f>
+        <v>3</v>
+      </c>
+      <c r="L28">
+        <f>IF(F28&lt;20, 1, IF(F28&lt;30,2,IF(F28&lt;45,3,4)))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -1580,8 +1835,16 @@
       <c r="J29">
         <v>23</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K29">
+        <f>IF(E29&lt;10, 1, IF(E29&lt;15,2,IF(E29&lt;20,3,4)))</f>
+        <v>3</v>
+      </c>
+      <c r="L29">
+        <f>IF(F29&lt;20, 1, IF(F29&lt;30,2,IF(F29&lt;45,3,4)))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -1612,28 +1875,36 @@
       <c r="J30">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K30">
+        <f>IF(E30&lt;10, 1, IF(E30&lt;15,2,IF(E30&lt;20,3,4)))</f>
+        <v>3</v>
+      </c>
+      <c r="L30">
+        <f>IF(F30&lt;20, 1, IF(F30&lt;30,2,IF(F30&lt;45,3,4)))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B31">
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="D31" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="E31">
         <v>18</v>
       </c>
       <c r="F31">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="G31">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="H31" t="s">
         <v>78</v>
@@ -1642,10 +1913,18 @@
         <v>64</v>
       </c>
       <c r="J31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="K31">
+        <f>IF(E31&lt;10, 1, IF(E31&lt;15,2,IF(E31&lt;20,3,4)))</f>
+        <v>3</v>
+      </c>
+      <c r="L31">
+        <f>IF(F31&lt;20, 1, IF(F31&lt;30,2,IF(F31&lt;45,3,4)))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -1653,13 +1932,13 @@
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D32" t="s">
         <v>72</v>
       </c>
       <c r="E32">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F32">
         <v>44</v>
@@ -1674,42 +1953,58 @@
         <v>64</v>
       </c>
       <c r="J32">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <f>IF(E32&lt;10, 1, IF(E32&lt;15,2,IF(E32&lt;20,3,4)))</f>
+        <v>3</v>
+      </c>
+      <c r="L32">
+        <f>IF(F32&lt;20, 1, IF(F32&lt;30,2,IF(F32&lt;45,3,4)))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D33" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E33">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F33">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="G33">
-        <v>700</v>
+        <v>400</v>
       </c>
       <c r="H33" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I33">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="J33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="K33">
+        <f>IF(E33&lt;10, 1, IF(E33&lt;15,2,IF(E33&lt;20,3,4)))</f>
+        <v>3</v>
+      </c>
+      <c r="L33">
+        <f>IF(F33&lt;20, 1, IF(F33&lt;30,2,IF(F33&lt;45,3,4)))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>25</v>
       </c>
@@ -1740,28 +2035,36 @@
       <c r="J34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K34">
+        <f>IF(E34&lt;10, 1, IF(E34&lt;15,2,IF(E34&lt;20,3,4)))</f>
+        <v>3</v>
+      </c>
+      <c r="L34">
+        <f>IF(F34&lt;20, 1, IF(F34&lt;30,2,IF(F34&lt;45,3,4)))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B35">
         <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="D35" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E35">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F35">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="G35">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="H35" t="s">
         <v>79</v>
@@ -1772,25 +2075,33 @@
       <c r="J35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K35">
+        <f>IF(E35&lt;10, 1, IF(E35&lt;15,2,IF(E35&lt;20,3,4)))</f>
+        <v>4</v>
+      </c>
+      <c r="L35">
+        <f>IF(F35&lt;20, 1, IF(F35&lt;30,2,IF(F35&lt;45,3,4)))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B36">
         <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="D36" t="s">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="E36">
         <v>20</v>
       </c>
       <c r="F36">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="G36">
         <v>500</v>
@@ -1804,25 +2115,33 @@
       <c r="J36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K36">
+        <f>IF(E36&lt;10, 1, IF(E36&lt;15,2,IF(E36&lt;20,3,4)))</f>
+        <v>4</v>
+      </c>
+      <c r="L36">
+        <f>IF(F36&lt;20, 1, IF(F36&lt;30,2,IF(F36&lt;45,3,4)))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B37">
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E37">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="F37">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G37">
         <v>500</v>
@@ -1834,30 +2153,38 @@
         <v>37</v>
       </c>
       <c r="J37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="K37">
+        <f>IF(E37&lt;10, 1, IF(E37&lt;15,2,IF(E37&lt;20,3,4)))</f>
+        <v>4</v>
+      </c>
+      <c r="L37">
+        <f>IF(F37&lt;20, 1, IF(F37&lt;30,2,IF(F37&lt;45,3,4)))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B38">
         <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="D38" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E38">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F38">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G38">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="H38" t="s">
         <v>79</v>
@@ -1866,10 +2193,18 @@
         <v>37</v>
       </c>
       <c r="J38">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="K38">
+        <f>IF(E38&lt;10, 1, IF(E38&lt;15,2,IF(E38&lt;20,3,4)))</f>
+        <v>4</v>
+      </c>
+      <c r="L38">
+        <f>IF(F38&lt;20, 1, IF(F38&lt;30,2,IF(F38&lt;45,3,4)))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>21</v>
       </c>
@@ -1877,16 +2212,16 @@
         <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D39" t="s">
         <v>21</v>
       </c>
       <c r="E39">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F39">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="G39">
         <v>400</v>
@@ -1900,8 +2235,16 @@
       <c r="J39">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K39">
+        <f>IF(E39&lt;10, 1, IF(E39&lt;15,2,IF(E39&lt;20,3,4)))</f>
+        <v>4</v>
+      </c>
+      <c r="L39">
+        <f>IF(F39&lt;20, 1, IF(F39&lt;30,2,IF(F39&lt;45,3,4)))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>21</v>
       </c>
@@ -1909,16 +2252,16 @@
         <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D40" t="s">
         <v>21</v>
       </c>
       <c r="E40">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F40">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="G40">
         <v>400</v>
@@ -1932,8 +2275,16 @@
       <c r="J40">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K40">
+        <f>IF(E40&lt;10, 1, IF(E40&lt;15,2,IF(E40&lt;20,3,4)))</f>
+        <v>4</v>
+      </c>
+      <c r="L40">
+        <f>IF(F40&lt;20, 1, IF(F40&lt;30,2,IF(F40&lt;45,3,4)))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>22</v>
       </c>
@@ -1941,16 +2292,16 @@
         <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D41" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="E41">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F41">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="G41">
         <v>400</v>
@@ -1962,27 +2313,35 @@
         <v>37</v>
       </c>
       <c r="J41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="K41">
+        <f>IF(E41&lt;10, 1, IF(E41&lt;15,2,IF(E41&lt;20,3,4)))</f>
+        <v>4</v>
+      </c>
+      <c r="L41">
+        <f>IF(F41&lt;20, 1, IF(F41&lt;30,2,IF(F41&lt;45,3,4)))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B42">
         <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="D42" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="E42">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="F42">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="G42">
         <v>500</v>
@@ -1996,11 +2355,19 @@
       <c r="J42">
         <v>1</v>
       </c>
+      <c r="K42">
+        <f>IF(E42&lt;10, 1, IF(E42&lt;15,2,IF(E42&lt;20,3,4)))</f>
+        <v>4</v>
+      </c>
+      <c r="L42">
+        <f>IF(F42&lt;20, 1, IF(F42&lt;30,2,IF(F42&lt;45,3,4)))</f>
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J42" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J42">
-      <sortCondition ref="E1:E42"/>
+  <autoFilter ref="A1:L43" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L43">
+      <sortCondition ref="K1:K43"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>